<commit_message>
Added natural or laboratory hybridization
</commit_message>
<xml_diff>
--- a/Windows/Busquedas/WebOfScience/Hybrid/Diptera/Diptera_Hybrids.xlsx
+++ b/Windows/Busquedas/WebOfScience/Hybrid/Diptera/Diptera_Hybrids.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Eureka" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hybrids!$A$1:$E$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hybrids!$A$1:$F$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="254">
   <si>
     <t>Sp1</t>
   </si>
@@ -227,12 +227,6 @@
     <t>Mishra, PK; Singh, BN.</t>
   </si>
   <si>
-    <t>Michailova, P.</t>
-  </si>
-  <si>
-    <t>Cytogenetic analysis of a hybrid, Glyptotendipes pallens Mg. x Glyptotendipes glaucus Mg. (Diptera, Chironomidae): evolutionary considerations</t>
-  </si>
-  <si>
     <t>Hybridization between two polyphagous fruit-fly species (Diptera : Tephritidae) causes sex-biased reduction in developmental stability</t>
   </si>
   <si>
@@ -777,6 +771,27 @@
   </si>
   <si>
     <t>Savage, HM.</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Rull, J; Tadeo, E; Lasa, R; Rodriguez, CL; Altuzar-Molina, A; Aluja, M.</t>
+  </si>
+  <si>
+    <t>Experimental hybridization and reproductive isolation between two sympatric species of tephritid fruit flies in the Anastrepha fraterculus species group</t>
+  </si>
+  <si>
+    <t>Michailova, P; Warchalowska-Sliwa, E; Kownacki, A.</t>
+  </si>
+  <si>
+    <t>Cytotaxonomic characteristics of the genus Glyptotendipes Kieffer (Chironomidae, Diptera) from fish and retention ponds (Silesia, southern Poland)</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1129,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,11 +1155,12 @@
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1155,13 +1171,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1171,14 +1190,17 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2">
         <v>2019</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1188,14 +1210,17 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3">
         <v>2013</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1205,14 +1230,17 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4">
         <v>1996</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1222,14 +1250,17 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5">
         <v>2001</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1239,14 +1270,17 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6">
         <v>2001</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1254,16 +1288,19 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>2001</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="D7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1273,14 +1310,17 @@
       <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8">
         <v>2007</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1290,14 +1330,17 @@
       <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9">
         <v>2005</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1307,14 +1350,17 @@
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10">
         <v>1997</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1324,14 +1370,17 @@
       <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11">
         <v>2013</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1341,14 +1390,17 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>248</v>
+      </c>
+      <c r="E12">
         <v>2000</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1358,14 +1410,17 @@
       <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13">
         <v>2013</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1375,14 +1430,17 @@
       <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14">
         <v>2003</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1392,14 +1450,17 @@
       <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15">
         <v>2014</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1409,14 +1470,17 @@
       <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16">
         <v>2008</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1424,680 +1488,797 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17">
-        <v>1998</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="D17" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17">
+        <v>2001</v>
+      </c>
+      <c r="F17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E18">
+        <v>2014</v>
+      </c>
+      <c r="F18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="D18">
-        <v>2014</v>
-      </c>
-      <c r="E18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>248</v>
+      </c>
+      <c r="E19">
+        <v>2020</v>
+      </c>
+      <c r="F19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="D19">
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>248</v>
+      </c>
+      <c r="E20">
+        <v>2019</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21">
+        <v>2019</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>249</v>
+      </c>
+      <c r="E23">
+        <v>2019</v>
+      </c>
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>249</v>
+      </c>
+      <c r="E24">
+        <v>2009</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>249</v>
+      </c>
+      <c r="E25">
+        <v>2010</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E26">
+        <v>2008</v>
+      </c>
+      <c r="F26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" t="s">
+        <v>248</v>
+      </c>
+      <c r="E27">
+        <v>1995</v>
+      </c>
+      <c r="F27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>248</v>
+      </c>
+      <c r="E28">
+        <v>2002</v>
+      </c>
+      <c r="F28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29">
+        <v>2004</v>
+      </c>
+      <c r="F29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30">
         <v>2020</v>
       </c>
-      <c r="E19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20">
-        <v>2019</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21">
-        <v>2019</v>
-      </c>
-      <c r="E21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23">
-        <v>2019</v>
-      </c>
-      <c r="E23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24">
-        <v>2009</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25">
-        <v>2010</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26">
-        <v>2008</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27">
-        <v>1995</v>
-      </c>
-      <c r="E27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28">
-        <v>2002</v>
-      </c>
-      <c r="E28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29">
-        <v>2004</v>
-      </c>
-      <c r="E29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="F30" t="s">
         <v>117</v>
       </c>
-      <c r="B30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
-        <v>2020</v>
-      </c>
-      <c r="E30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
       <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31">
+        <v>2001</v>
+      </c>
+      <c r="F31" t="s">
         <v>121</v>
       </c>
-      <c r="C31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31">
-        <v>2001</v>
-      </c>
-      <c r="E31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
         <v>128</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
         <v>129</v>
       </c>
-      <c r="D32" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="C33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
+        <v>248</v>
+      </c>
+      <c r="E33">
+        <v>2020</v>
+      </c>
+      <c r="F33" t="s">
         <v>131</v>
       </c>
-      <c r="C33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33">
-        <v>2020</v>
-      </c>
-      <c r="E33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
         <v>136</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34">
+        <v>1982</v>
+      </c>
+      <c r="F34" t="s">
         <v>137</v>
       </c>
-      <c r="C34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34">
-        <v>1982</v>
-      </c>
-      <c r="E34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35">
+        <v>138</v>
+      </c>
+      <c r="D35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E35">
         <v>2018</v>
       </c>
-      <c r="E35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" t="s">
         <v>144</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
+        <v>249</v>
+      </c>
+      <c r="E36">
+        <v>2006</v>
+      </c>
+      <c r="F36" t="s">
         <v>145</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>146</v>
       </c>
-      <c r="D36">
-        <v>2006</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B37" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>248</v>
+      </c>
+      <c r="E37">
+        <v>1984</v>
+      </c>
+      <c r="F37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
         <v>148</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>149</v>
       </c>
-      <c r="C37" t="s">
-        <v>151</v>
-      </c>
-      <c r="D37">
+      <c r="D38" t="s">
+        <v>248</v>
+      </c>
+      <c r="E38">
         <v>1984</v>
       </c>
-      <c r="E37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F38" t="s">
         <v>150</v>
       </c>
-      <c r="C38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D38">
-        <v>1984</v>
-      </c>
-      <c r="E38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" t="s">
         <v>155</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
+        <v>249</v>
+      </c>
+      <c r="E39">
+        <v>1995</v>
+      </c>
+      <c r="F39" t="s">
         <v>156</v>
       </c>
-      <c r="C39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E40">
+        <v>2018</v>
+      </c>
+      <c r="F40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41">
         <v>1995</v>
       </c>
-      <c r="E39" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>165</v>
-      </c>
-      <c r="B40" t="s">
-        <v>166</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="F41" t="s">
         <v>167</v>
       </c>
-      <c r="D40">
-        <v>2018</v>
-      </c>
-      <c r="E40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>171</v>
-      </c>
-      <c r="B41" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" t="s">
-        <v>170</v>
-      </c>
-      <c r="D41">
-        <v>1995</v>
-      </c>
-      <c r="E41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" t="s">
         <v>179</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
+        <v>248</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" t="s">
         <v>180</v>
       </c>
-      <c r="C42" t="s">
-        <v>181</v>
-      </c>
-      <c r="D42" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" t="s">
         <v>187</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
+        <v>249</v>
+      </c>
+      <c r="E43">
+        <v>1997</v>
+      </c>
+      <c r="F43" t="s">
         <v>188</v>
       </c>
-      <c r="C43" t="s">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>189</v>
       </c>
-      <c r="D43">
+      <c r="B44" t="s">
+        <v>190</v>
+      </c>
+      <c r="C44" t="s">
+        <v>191</v>
+      </c>
+      <c r="D44" t="s">
+        <v>248</v>
+      </c>
+      <c r="E44">
+        <v>2004</v>
+      </c>
+      <c r="F44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" t="s">
+        <v>248</v>
+      </c>
+      <c r="E45">
+        <v>2013</v>
+      </c>
+      <c r="F45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C46" t="s">
+        <v>199</v>
+      </c>
+      <c r="D46" t="s">
+        <v>248</v>
+      </c>
+      <c r="E46">
+        <v>2016</v>
+      </c>
+      <c r="F46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47">
+        <v>2015</v>
+      </c>
+      <c r="F47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48" t="s">
+        <v>206</v>
+      </c>
+      <c r="C48" t="s">
+        <v>208</v>
+      </c>
+      <c r="D48" t="s">
+        <v>249</v>
+      </c>
+      <c r="E48">
+        <v>2008</v>
+      </c>
+      <c r="F48" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>209</v>
+      </c>
+      <c r="B49" t="s">
+        <v>210</v>
+      </c>
+      <c r="C49" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" t="s">
+        <v>249</v>
+      </c>
+      <c r="E49">
+        <v>2014</v>
+      </c>
+      <c r="F49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" t="s">
+        <v>249</v>
+      </c>
+      <c r="E50">
+        <v>1991</v>
+      </c>
+      <c r="F50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>219</v>
+      </c>
+      <c r="B51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" t="s">
+        <v>221</v>
+      </c>
+      <c r="D51" t="s">
+        <v>249</v>
+      </c>
+      <c r="E51">
+        <v>1998</v>
+      </c>
+      <c r="F51" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>223</v>
+      </c>
+      <c r="B52" t="s">
+        <v>224</v>
+      </c>
+      <c r="C52" t="s">
+        <v>225</v>
+      </c>
+      <c r="D52" t="s">
+        <v>249</v>
+      </c>
+      <c r="E52">
+        <v>1989</v>
+      </c>
+      <c r="F52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53" t="s">
+        <v>229</v>
+      </c>
+      <c r="D53" t="s">
+        <v>248</v>
+      </c>
+      <c r="E53">
+        <v>2020</v>
+      </c>
+      <c r="F53" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" t="s">
+        <v>233</v>
+      </c>
+      <c r="D54" t="s">
+        <v>249</v>
+      </c>
+      <c r="E54">
+        <v>1999</v>
+      </c>
+      <c r="F54" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>237</v>
+      </c>
+      <c r="B55" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" t="s">
+        <v>248</v>
+      </c>
+      <c r="E55">
+        <v>1981</v>
+      </c>
+      <c r="F55" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" t="s">
+        <v>249</v>
+      </c>
+      <c r="E56">
         <v>1997</v>
       </c>
-      <c r="E43" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>191</v>
-      </c>
-      <c r="B44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" t="s">
-        <v>193</v>
-      </c>
-      <c r="D44">
-        <v>2004</v>
-      </c>
-      <c r="E44" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" t="s">
-        <v>197</v>
-      </c>
-      <c r="C45" t="s">
-        <v>196</v>
-      </c>
-      <c r="D45">
-        <v>2013</v>
-      </c>
-      <c r="E45" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D46">
-        <v>2016</v>
-      </c>
-      <c r="E46" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>203</v>
-      </c>
-      <c r="B47" t="s">
-        <v>204</v>
-      </c>
-      <c r="C47" t="s">
-        <v>205</v>
-      </c>
-      <c r="D47">
-        <v>2015</v>
-      </c>
-      <c r="E47" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>207</v>
-      </c>
-      <c r="B48" t="s">
-        <v>208</v>
-      </c>
-      <c r="C48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48">
-        <v>2008</v>
-      </c>
-      <c r="E48" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>211</v>
-      </c>
-      <c r="B49" t="s">
-        <v>212</v>
-      </c>
-      <c r="C49" t="s">
-        <v>213</v>
-      </c>
-      <c r="D49">
-        <v>2014</v>
-      </c>
-      <c r="E49" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>215</v>
-      </c>
-      <c r="B50" t="s">
-        <v>216</v>
-      </c>
-      <c r="C50" t="s">
-        <v>217</v>
-      </c>
-      <c r="D50">
-        <v>1991</v>
-      </c>
-      <c r="E50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" t="s">
-        <v>222</v>
-      </c>
-      <c r="C51" t="s">
-        <v>223</v>
-      </c>
-      <c r="D51">
-        <v>1998</v>
-      </c>
-      <c r="E51" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>225</v>
-      </c>
-      <c r="B52" t="s">
-        <v>226</v>
-      </c>
-      <c r="C52" t="s">
-        <v>227</v>
-      </c>
-      <c r="D52">
-        <v>1989</v>
-      </c>
-      <c r="E52" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>131</v>
-      </c>
-      <c r="B53" t="s">
-        <v>128</v>
-      </c>
-      <c r="C53" t="s">
-        <v>231</v>
-      </c>
-      <c r="D53">
-        <v>2020</v>
-      </c>
-      <c r="E53" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>233</v>
-      </c>
-      <c r="B54" t="s">
-        <v>234</v>
-      </c>
-      <c r="C54" t="s">
-        <v>235</v>
-      </c>
-      <c r="D54">
-        <v>1999</v>
-      </c>
-      <c r="E54" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>239</v>
-      </c>
-      <c r="B55" t="s">
-        <v>240</v>
-      </c>
-      <c r="C55" t="s">
-        <v>241</v>
-      </c>
-      <c r="D55">
-        <v>1981</v>
-      </c>
-      <c r="E55" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>243</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="F56" t="s">
         <v>244</v>
       </c>
-      <c r="C56" t="s">
-        <v>245</v>
-      </c>
-      <c r="D56">
-        <v>1997</v>
-      </c>
-      <c r="E56" t="s">
-        <v>246</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E56"/>
+  <autoFilter ref="A1:F56"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2151,211 +2332,211 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>2008</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5">
         <v>2006</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B6">
         <v>2009</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>2008</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8">
         <v>2014</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9">
         <v>1990</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B10">
         <v>1991</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B11">
         <v>1980</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B12">
         <v>2007</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13">
         <v>2016</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B14">
         <v>2002</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B15">
         <v>2012</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16">
         <v>1999</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B17">
         <v>2018</v>
       </c>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B18">
         <v>1983</v>
       </c>
       <c r="C18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B19">
         <v>1987</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B20">
         <v>1992</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B21">
         <v>1987</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B22">
         <v>2006</v>
       </c>
       <c r="C22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2367,7 +2548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2386,13 +2567,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>